<commit_message>
Stock plan generator implemented.
</commit_message>
<xml_diff>
--- a/assets/templates/ff_beru_supply.xlsx
+++ b/assets/templates/ff_beru_supply.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Поставка" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="472">
   <si>
     <t xml:space="preserve">Ваш SKU</t>
   </si>
@@ -282,6 +282,216 @@
     <t xml:space="preserve">48330015300506</t>
   </si>
   <si>
+    <t xml:space="preserve">2000344410006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, белый, ярко-зеленый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000344410020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, светло-зеленый, сиреневый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, бирюзовый, желтый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, бирюзовый, сиреневый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, бордовый, бирюзовый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, бордовый. желтый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, малиновый, желтый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, малиновый, сиреневый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, розовый, бирюзовый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, розовый, бордовый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, розовый, желтый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, розовый, светло-голубой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000396857101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, сиреневый, желтый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, белый, светло-кремовый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, белый, темно-синий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, белый, оранжевый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, васильковый, красный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, васильковый. лимонный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, васильковый, лимонный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, красный, темно-синий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, красный. лимонный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, лимонный, темно-синий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, лимонный, персиковый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, лимонный, оранжевый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, персиковый, светло-кремовый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467357165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, светло-кремовый, темно-синий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467476002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, белый, красный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467476019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, белый, лимонный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467476026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, светло-зеленый, красный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467476033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, светло-зеленый, лимонный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467476040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, светло-зеленый, оранжевый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467476057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, светло-зеленый, пресиковый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467476071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, светло-зеленый, темно-синий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000467502008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, белый, светло-зеленый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000572314008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплект полотенец 70x140, 2 шт, оранжевый, сиреневый</t>
+  </si>
+  <si>
     <t xml:space="preserve">48330015300492</t>
   </si>
   <si>
@@ -348,10 +558,19 @@
     <t xml:space="preserve">Полотенце шоколад 50x90</t>
   </si>
   <si>
+    <t xml:space="preserve">48330015300634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Полотенце ярко-зеленое 70x140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Полотенце голубой 70x140</t>
+  </si>
+  <si>
     <t xml:space="preserve">48330015300645</t>
   </si>
   <si>
-    <t xml:space="preserve">Полотенце лимонный 70x140</t>
+    <t xml:space="preserve">Полотенце лимонное 70x140</t>
   </si>
   <si>
     <t xml:space="preserve">48330015300646</t>
@@ -363,15 +582,12 @@
     <t xml:space="preserve">48330015300647</t>
   </si>
   <si>
-    <t xml:space="preserve">Полотенце малиновый 70x140</t>
+    <t xml:space="preserve">Полотенце малиновое 70x140</t>
   </si>
   <si>
     <t xml:space="preserve">48330015300648</t>
   </si>
   <si>
-    <t xml:space="preserve">Полотенце зеленый 70x140</t>
-  </si>
-  <si>
     <t xml:space="preserve">48330015300649</t>
   </si>
   <si>
@@ -387,19 +603,25 @@
     <t xml:space="preserve">48330015300651</t>
   </si>
   <si>
-    <t xml:space="preserve">Полотенце розовый 70x140</t>
+    <t xml:space="preserve">Полотенце розовое 70x140</t>
   </si>
   <si>
     <t xml:space="preserve">48330015300652</t>
   </si>
   <si>
-    <t xml:space="preserve">Полотенце светло-зеленый 70x140</t>
+    <t xml:space="preserve">Полотенце светло-зеленое 70x140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48330015300653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Полотенце темно-оливковое 70x140</t>
   </si>
   <si>
     <t xml:space="preserve">48330015300654</t>
   </si>
   <si>
-    <t xml:space="preserve">Полотенце темно-синий 70x140</t>
+    <t xml:space="preserve">Полотенце темно-синее 70x140</t>
   </si>
   <si>
     <t xml:space="preserve">48330015300701</t>
@@ -1623,23 +1845,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J170"/>
+  <dimension ref="A1:H220"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A95" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="19.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="19.61"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="19.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="19.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="27.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1653,24 +1871,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1684,16 +1896,7 @@
       <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1707,16 +1910,7 @@
       <c r="C3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1730,16 +1924,7 @@
       <c r="C4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1753,16 +1938,7 @@
       <c r="C5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0" t="n">
+      <c r="E5" s="0" t="n">
         <v>195</v>
       </c>
     </row>
@@ -1776,16 +1952,7 @@
       <c r="C6" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="E6" s="0" t="n">
         <v>197</v>
       </c>
     </row>
@@ -1799,16 +1966,7 @@
       <c r="C7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="E7" s="0" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1822,16 +1980,7 @@
       <c r="C8" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1845,14 +1994,8 @@
       <c r="C9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>0</v>
+      <c r="E9" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,16 +2008,7 @@
       <c r="C10" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1888,14 +2022,8 @@
       <c r="C11" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>0</v>
+      <c r="E11" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,16 +2036,7 @@
       <c r="C12" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1931,16 +2050,7 @@
       <c r="C13" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1954,17 +2064,8 @@
       <c r="C14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>197</v>
+      <c r="E14" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1977,16 +2078,7 @@
       <c r="C15" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="0" t="n">
+      <c r="E15" s="0" t="n">
         <v>203</v>
       </c>
     </row>
@@ -2000,16 +2092,7 @@
       <c r="C16" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -2023,16 +2106,7 @@
       <c r="C17" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="0" t="n">
+      <c r="E17" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -2046,16 +2120,7 @@
       <c r="C18" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="0" t="n">
+      <c r="E18" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -2069,16 +2134,7 @@
       <c r="C19" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="0" t="n">
+      <c r="E19" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -2092,16 +2148,7 @@
       <c r="C20" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G20" s="0" t="n">
+      <c r="E20" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -2115,16 +2162,7 @@
       <c r="C21" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="0" t="n">
+      <c r="E21" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -2138,16 +2176,7 @@
       <c r="C22" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="0" t="n">
+      <c r="E22" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -2161,16 +2190,7 @@
       <c r="C23" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="0" t="n">
+      <c r="E23" s="0" t="n">
         <v>90</v>
       </c>
     </row>
@@ -2184,16 +2204,7 @@
       <c r="C24" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="0" t="n">
+      <c r="E24" s="0" t="n">
         <v>90</v>
       </c>
     </row>
@@ -2207,15 +2218,6 @@
       <c r="C25" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -2227,16 +2229,7 @@
       <c r="C26" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="0" t="n">
+      <c r="E26" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -2250,16 +2243,7 @@
       <c r="C27" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="0" t="n">
+      <c r="E27" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -2273,15 +2257,6 @@
       <c r="C28" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -2293,15 +2268,6 @@
       <c r="C29" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -2313,15 +2279,6 @@
       <c r="C30" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F30" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -2333,15 +2290,6 @@
       <c r="C31" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -2353,15 +2301,6 @@
       <c r="C32" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
@@ -2373,15 +2312,6 @@
       <c r="C33" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -2393,15 +2323,6 @@
       <c r="C34" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -2413,15 +2334,6 @@
       <c r="C35" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -2433,15 +2345,6 @@
       <c r="C36" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -2453,15 +2356,6 @@
       <c r="C37" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
@@ -2473,15 +2367,6 @@
       <c r="C38" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
@@ -2493,18 +2378,6 @@
       <c r="C39" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="0" t="n">
-        <v>200</v>
-      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
@@ -2516,15 +2389,6 @@
       <c r="C40" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -2536,18 +2400,6 @@
       <c r="C41" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="0" t="n">
-        <v>200</v>
-      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -2559,18 +2411,6 @@
       <c r="C42" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" s="0" t="n">
-        <v>200</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -2582,18 +2422,6 @@
       <c r="C43" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <v>200</v>
-      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -2605,15 +2433,6 @@
       <c r="C44" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -2625,15 +2444,6 @@
       <c r="C45" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -2645,18 +2455,6 @@
       <c r="C46" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" s="0" t="n">
-        <v>200</v>
-      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -2668,18 +2466,6 @@
       <c r="C47" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="F47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G47" s="0" t="n">
-        <v>200</v>
-      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
@@ -2691,15 +2477,6 @@
       <c r="C48" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -2711,15 +2488,6 @@
       <c r="C49" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -2731,15 +2499,6 @@
       <c r="C50" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F50" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
@@ -2751,15 +2510,6 @@
       <c r="C51" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="F51" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
@@ -2771,15 +2521,6 @@
       <c r="C52" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="F52" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
@@ -2791,15 +2532,6 @@
       <c r="C53" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D53" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
@@ -2811,15 +2543,6 @@
       <c r="C54" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="D54" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="F54" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
@@ -2831,15 +2554,6 @@
       <c r="C55" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="D55" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="F55" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
@@ -2851,15 +2565,6 @@
       <c r="C56" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D56" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F56" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
@@ -2871,15 +2576,6 @@
       <c r="C57" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="D57" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F57" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
@@ -2891,15 +2587,6 @@
       <c r="C58" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="F58" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
@@ -2911,15 +2598,6 @@
       <c r="C59" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F59" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
@@ -2931,15 +2609,6 @@
       <c r="C60" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="F60" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
@@ -2951,15 +2620,6 @@
       <c r="C61" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="D61" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="F61" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
@@ -2971,15 +2631,6 @@
       <c r="C62" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="D62" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="F62" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
@@ -2991,15 +2642,6 @@
       <c r="C63" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="F63" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
@@ -3011,15 +2653,6 @@
       <c r="C64" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="D64" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="F64" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
@@ -3031,15 +2664,6 @@
       <c r="C65" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="D65" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="F65" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
@@ -3051,15 +2675,6 @@
       <c r="C66" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="D66" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="F66" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
@@ -3071,15 +2686,6 @@
       <c r="C67" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="D67" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="F67" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
@@ -3091,15 +2697,6 @@
       <c r="C68" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="D68" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="F68" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
@@ -3111,15 +2708,6 @@
       <c r="C69" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="D69" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="F69" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
@@ -3131,15 +2719,6 @@
       <c r="C70" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="D70" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="F70" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
@@ -3151,15 +2730,6 @@
       <c r="C71" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="D71" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="F71" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
@@ -3171,15 +2741,6 @@
       <c r="C72" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="D72" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="F72" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
@@ -3191,2068 +2752,1814 @@
       <c r="C73" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="D73" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>178</v>
+        <v>25</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>179</v>
+        <v>24</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="F74" s="0" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>180</v>
+        <v>10</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="F75" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>182</v>
+        <v>31</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>183</v>
+        <v>30</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="F76" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G76" s="0" t="n">
-        <v>650</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="F77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G77" s="0" t="n">
-        <v>670</v>
+        <v>178</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>186</v>
+        <v>34</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>187</v>
+        <v>33</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="F78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G78" s="0" t="n">
-        <v>670</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>188</v>
+        <v>13</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>189</v>
+        <v>12</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="F79" s="0" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>190</v>
+        <v>16</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="F80" s="0" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>192</v>
+        <v>19</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>193</v>
+        <v>18</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="E81" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="F81" s="0" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>194</v>
+        <v>28</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>195</v>
+        <v>27</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="F82" s="0" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>196</v>
+        <v>37</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E83" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F83" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G83" s="0" t="n">
-        <v>670</v>
+        <v>37</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>198</v>
+        <v>49</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>199</v>
+        <v>48</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="F84" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G84" s="0" t="n">
-        <v>700</v>
+        <v>49</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>201</v>
+        <v>39</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="E85" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="F85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G85" s="0" t="n">
-        <v>700</v>
+        <v>40</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>202</v>
+        <v>46</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>203</v>
+        <v>45</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="E86" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="F86" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G86" s="0" t="n">
-        <v>700</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>204</v>
+        <v>43</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>205</v>
+        <v>42</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="F87" s="0" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="E88" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="F88" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G88" s="0" t="n">
-        <v>700</v>
+        <v>181</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="D89" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="E89" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="F89" s="0" t="n">
-        <v>0</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="E90" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="F90" s="0" t="n">
-        <v>0</v>
+        <v>185</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>213</v>
+        <v>21</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="D91" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="E91" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="F91" s="0" t="n">
-        <v>0</v>
+        <v>187</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>215</v>
+        <v>189</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="D92" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="F92" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G92" s="0" t="n">
-        <v>700</v>
+        <v>188</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="E93" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="F93" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G93" s="0" t="n">
-        <v>800</v>
+        <v>190</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="E94" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="F94" s="0" t="n">
-        <v>0</v>
+        <v>192</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="E95" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="F95" s="0" t="n">
-        <v>0</v>
+        <v>194</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="E96" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="F96" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G96" s="0" t="n">
-        <v>800</v>
+        <v>196</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="E97" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="F97" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G97" s="0" t="n">
-        <v>800</v>
+        <v>198</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="D98" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="E98" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="F98" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G98" s="0" t="n">
-        <v>800</v>
+        <v>200</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="D99" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="E99" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="F99" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G99" s="0" t="n">
-        <v>800</v>
+        <v>202</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="D100" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="E100" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="F100" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G100" s="0" t="n">
-        <v>800</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="E101" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="F101" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G101" s="0" t="n">
-        <v>800</v>
+        <v>206</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="E102" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="F102" s="0" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>236</v>
+        <v>210</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>237</v>
+        <v>211</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="D103" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="E103" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="F103" s="0" t="n">
-        <v>0</v>
+        <v>210</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="D104" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="E104" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="F104" s="0" t="n">
-        <v>0</v>
+        <v>212</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="D105" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="E105" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="F105" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G105" s="0" t="n">
-        <v>800</v>
+        <v>214</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="D106" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="E106" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="F106" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G106" s="0" t="n">
-        <v>800</v>
+        <v>216</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="D107" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="E107" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="F107" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G107" s="0" t="n">
-        <v>800</v>
+        <v>218</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="D108" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="E108" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="F108" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G108" s="0" t="n">
-        <v>800</v>
+        <v>220</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="D109" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="E109" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="F109" s="0" t="n">
-        <v>0</v>
+        <v>222</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="D110" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="E110" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="F110" s="0" t="n">
-        <v>0</v>
+        <v>224</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="D111" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="E111" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="F111" s="0" t="n">
-        <v>0</v>
+        <v>226</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="D112" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="E112" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="F112" s="0" t="n">
-        <v>0</v>
+        <v>228</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="D113" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="E113" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="F113" s="0" t="n">
-        <v>0</v>
+        <v>230</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="D114" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="E114" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="F114" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G114" s="0" t="n">
-        <v>800</v>
+        <v>232</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="D115" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="E115" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="F115" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G115" s="0" t="n">
-        <v>800</v>
+        <v>234</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="D116" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="E116" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="F116" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G116" s="0" t="n">
-        <v>279</v>
+        <v>236</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="D117" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="E117" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="F117" s="0" t="n">
-        <v>0</v>
+        <v>238</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="D118" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="E118" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="F118" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G118" s="0" t="n">
-        <v>300</v>
+        <v>240</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="E119" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="F119" s="0" t="n">
-        <v>0</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="D120" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="E120" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="F120" s="0" t="n">
-        <v>0</v>
+        <v>244</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="D121" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="E121" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="F121" s="0" t="n">
-        <v>0</v>
+        <v>246</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="D122" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="E122" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="F122" s="0" t="n">
-        <v>0</v>
+        <v>248</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="D123" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="E123" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="F123" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G123" s="0" t="n">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>279</v>
+        <v>253</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="D124" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="E124" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F124" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G124" s="0" t="n">
-        <v>300</v>
+        <v>252</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="D125" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="E125" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="F125" s="0" t="n">
-        <v>0</v>
+        <v>254</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>282</v>
+        <v>256</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="D126" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="E126" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="F126" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G126" s="0" t="n">
-        <v>290</v>
+        <v>256</v>
+      </c>
+      <c r="E126" s="0" t="n">
+        <v>600</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="D127" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="E127" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="F127" s="0" t="n">
-        <v>0</v>
+        <v>258</v>
+      </c>
+      <c r="E127" s="0" t="n">
+        <v>600</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="D128" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="E128" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="F128" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G128" s="0" t="n">
-        <v>300</v>
+        <v>260</v>
+      </c>
+      <c r="E128" s="0" t="n">
+        <v>670</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="D129" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="E129" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="F129" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G129" s="0" t="n">
-        <v>300</v>
+        <v>262</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="D130" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="E130" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F130" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G130" s="0" t="n">
-        <v>300</v>
+        <v>264</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="D131" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="E131" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="F131" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G131" s="0" t="n">
-        <v>300</v>
+        <v>266</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="D132" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="E132" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="F132" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G132" s="0" t="n">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>296</v>
+        <v>270</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="D133" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="E133" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="F133" s="0" t="n">
-        <v>0</v>
+        <v>270</v>
+      </c>
+      <c r="E133" s="0" t="n">
+        <v>670</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>298</v>
+        <v>272</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="D134" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="E134" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="F134" s="0" t="n">
-        <v>0</v>
+        <v>272</v>
+      </c>
+      <c r="E134" s="0" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="D135" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="E135" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="F135" s="0" t="n">
-        <v>0</v>
+        <v>274</v>
+      </c>
+      <c r="E135" s="0" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>302</v>
+        <v>276</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="D136" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="E136" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="F136" s="0" t="n">
-        <v>0</v>
+        <v>276</v>
+      </c>
+      <c r="E136" s="0" t="n">
+        <v>620</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>304</v>
+        <v>278</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="D137" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="E137" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="F137" s="0" t="n">
-        <v>0</v>
+        <v>278</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>306</v>
+        <v>280</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="D138" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="E138" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="F138" s="0" t="n">
-        <v>0</v>
+        <v>280</v>
+      </c>
+      <c r="E138" s="0" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="D139" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="E139" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="F139" s="0" t="n">
-        <v>0</v>
+        <v>282</v>
+      </c>
+      <c r="E139" s="0" t="n">
+        <v>680</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>311</v>
+        <v>285</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="D140" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="E140" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="F140" s="0" t="n">
-        <v>0</v>
+        <v>284</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>312</v>
+        <v>286</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>313</v>
+        <v>287</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="D141" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="E141" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="F141" s="0" t="n">
-        <v>0</v>
+        <v>286</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>314</v>
+        <v>288</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>315</v>
+        <v>289</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="D142" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="E142" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="F142" s="0" t="n">
-        <v>0</v>
+        <v>288</v>
+      </c>
+      <c r="E142" s="0" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>317</v>
+        <v>291</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="D143" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="E143" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="F143" s="0" t="n">
-        <v>0</v>
+        <v>290</v>
+      </c>
+      <c r="E143" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="D144" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="E144" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="F144" s="0" t="n">
-        <v>0</v>
+        <v>292</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="D145" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="E145" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="F145" s="0" t="n">
-        <v>0</v>
+        <v>294</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>322</v>
+        <v>296</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>323</v>
+        <v>297</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="D146" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="E146" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="F146" s="0" t="n">
-        <v>0</v>
+        <v>296</v>
+      </c>
+      <c r="E146" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>324</v>
+        <v>298</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>325</v>
+        <v>299</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="D147" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="E147" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="F147" s="0" t="n">
-        <v>0</v>
+        <v>298</v>
+      </c>
+      <c r="E147" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>327</v>
+        <v>301</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="D148" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="E148" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="F148" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
+      </c>
+      <c r="E148" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>328</v>
+        <v>302</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="D149" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="E149" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="F149" s="0" t="n">
-        <v>0</v>
+        <v>302</v>
+      </c>
+      <c r="E149" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="D150" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="E150" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="F150" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G150" s="0" t="n">
-        <v>174</v>
+        <v>304</v>
+      </c>
+      <c r="E150" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>332</v>
+        <v>306</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="D151" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="E151" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="F151" s="0" t="n">
-        <v>0</v>
+        <v>306</v>
+      </c>
+      <c r="E151" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D152" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E152" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="F152" s="0" t="n">
-        <v>0</v>
+        <v>308</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>336</v>
+        <v>310</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="D153" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="E153" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="F153" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G153" s="0" t="n">
-        <v>174</v>
+        <v>310</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>339</v>
+        <v>313</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="D154" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="E154" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="F154" s="0" t="n">
-        <v>0</v>
+        <v>312</v>
+      </c>
+      <c r="E154" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="D155" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="E155" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="F155" s="0" t="n">
-        <v>0</v>
+        <v>314</v>
+      </c>
+      <c r="E155" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="D156" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="E156" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="F156" s="0" t="n">
-        <v>0</v>
+        <v>316</v>
+      </c>
+      <c r="E156" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>345</v>
+        <v>319</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="D157" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="E157" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="F157" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G157" s="0" t="n">
-        <v>174</v>
+        <v>318</v>
+      </c>
+      <c r="E157" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="D158" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="E158" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="F158" s="0" t="n">
-        <v>0</v>
+        <v>320</v>
+      </c>
+      <c r="E158" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>348</v>
+        <v>322</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="D159" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="E159" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="F159" s="0" t="n">
-        <v>0</v>
+        <v>322</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="D160" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="E160" s="0" t="s">
-        <v>351</v>
-      </c>
-      <c r="F160" s="0" t="n">
-        <v>0</v>
+        <v>324</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="D161" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="E161" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="F161" s="0" t="n">
-        <v>0</v>
+        <v>326</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="D162" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="E162" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="F162" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G162" s="0" t="n">
-        <v>180</v>
+        <v>328</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="D163" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="E163" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="F163" s="0" t="n">
-        <v>0</v>
+        <v>330</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="D164" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="E164" s="0" t="s">
-        <v>359</v>
-      </c>
-      <c r="F164" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G164" s="0" t="n">
-        <v>174</v>
+        <v>332</v>
+      </c>
+      <c r="E164" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>360</v>
+        <v>334</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="D165" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="E165" s="0" t="s">
-        <v>361</v>
-      </c>
-      <c r="F165" s="0" t="n">
-        <v>0</v>
+        <v>334</v>
+      </c>
+      <c r="E165" s="0" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>362</v>
+        <v>336</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>363</v>
+        <v>337</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="D166" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="E166" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="F166" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G166" s="0" t="n">
-        <v>174</v>
+        <v>336</v>
+      </c>
+      <c r="E166" s="0" t="n">
+        <v>279</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>365</v>
+        <v>339</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="D167" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="E167" s="0" t="s">
-        <v>365</v>
-      </c>
-      <c r="F167" s="0" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>366</v>
+        <v>340</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="D168" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="E168" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="F168" s="0" t="n">
-        <v>0</v>
+        <v>340</v>
+      </c>
+      <c r="E168" s="0" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>368</v>
+        <v>342</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="D169" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="E169" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="F169" s="0" t="n">
-        <v>0</v>
+        <v>342</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="C171" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="C173" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E174" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="C176" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="E176" s="0" t="n">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="E178" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="C179" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="E179" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="C180" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="E180" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="C181" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="E181" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C182" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="E182" s="0" t="n">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="B170" s="0" t="s">
+      <c r="B183" s="0" t="s">
         <v>371</v>
       </c>
-      <c r="C170" s="0" t="s">
+      <c r="C183" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="D170" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="E170" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="F170" s="0" t="n">
-        <v>0</v>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C184" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C185" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="C186" s="0" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="C187" s="0" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="C188" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B189" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="C189" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="B190" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C190" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B191" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="C191" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="B192" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="C192" s="0" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B193" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="C193" s="0" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="B194" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="C194" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="C195" s="0" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="B196" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="C196" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C197" s="0" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="B198" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="C198" s="0" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="C199" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="C200" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E200" s="0" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="C201" s="0" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="E202" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="B203" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="C203" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E203" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="C204" s="0" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="C205" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="E205" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="C206" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="C207" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="E207" s="0" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="C208" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="E209" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="E210" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="B211" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="C211" s="0" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="C212" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="E212" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="C213" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C214" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="E214" s="0" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C215" s="0" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="B216" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="C216" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="E216" s="0" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C217" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="E217" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="C218" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="E218" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="B219" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="C219" s="0" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="B220" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C220" s="0" t="s">
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -5290,7 +4597,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="31.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>372</v>
+        <v>446</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -5300,19 +4607,19 @@
     </row>
     <row r="2" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>373</v>
+        <v>447</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>374</v>
+        <v>448</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>375</v>
+        <v>449</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>376</v>
+        <v>450</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>377</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="96.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5320,16 +4627,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>378</v>
+        <v>452</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>379</v>
+        <v>453</v>
       </c>
       <c r="D3" s="12" t="n">
         <v>4600728005002</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>380</v>
+        <v>454</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="58.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5338,13 +4645,13 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
-        <v>381</v>
+        <v>455</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>382</v>
+        <v>456</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>380</v>
+        <v>454</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5352,16 +4659,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>383</v>
+        <v>457</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>384</v>
+        <v>458</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>385</v>
+        <v>459</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>380</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5369,14 +4676,14 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>386</v>
+        <v>460</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>380</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5384,16 +4691,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>387</v>
+        <v>461</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>388</v>
+        <v>462</v>
       </c>
       <c r="D7" s="14" t="n">
         <v>229.08</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>380</v>
+        <v>454</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="124.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5401,16 +4708,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>389</v>
+        <v>463</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>390</v>
+        <v>464</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>391</v>
+        <v>465</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>380</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5418,14 +4725,14 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>392</v>
+        <v>466</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="11" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>393</v>
+        <v>467</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="31.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5433,16 +4740,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>394</v>
+        <v>468</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>395</v>
+        <v>469</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>396</v>
+        <v>470</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>397</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -5467,8 +4774,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5502,10 +4809,10 @@
       </c>
       <c r="B2" s="15" t="str">
         <f aca="false">INDEX(Поставка!$B:$B,MATCH(C2,Поставка!$C:$C,0))</f>
-        <v>Полотенце темно-синий 70x140</v>
+        <v>Полотенце темно-синее 70x140</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>124</v>
+        <v>198</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>9</v>
@@ -5521,7 +4828,7 @@
         <v>Полотенце 100x180 лимонный</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>152</v>
+        <v>226</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>4</v>
@@ -5537,7 +4844,7 @@
         <v>Простыня Байрамали махровая 150x210 красный</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>182</v>
+        <v>256</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>5</v>
@@ -5553,7 +4860,7 @@
         <v>Простыня Байрамали махровая 150x210 бирюзовый</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>208</v>
+        <v>282</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>10</v>
@@ -5569,7 +4876,7 @@
         <v>Простыня Байрамали махровая 180x210 бордовый</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>216</v>
+        <v>290</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>8</v>
@@ -5585,7 +4892,7 @@
         <v>Простыня Байрамали махровая 180x210 салатовый</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>228</v>
+        <v>302</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>10</v>
@@ -5601,7 +4908,7 @@
         <v>Простыня Байрамали махровая 180x210 светло-голубой</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>230</v>
+        <v>304</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>10</v>
@@ -5617,7 +4924,7 @@
         <v>Простыня Байрамали махровая 180x210 красный</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>238</v>
+        <v>312</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>5</v>
@@ -5633,7 +4940,7 @@
         <v>Простыня Байрамали махровая 180x210 лимонный</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>240</v>
+        <v>314</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>9</v>

</xml_diff>